<commit_message>
Eliminated to_string function in exchange for another 7-8% performance boost
SCPV2-1.4 is now about 15% faster than SCPV1-1.3/SCPV1-1.4. SCPV1-1.3 and SCPV1-1.4 are now about the same speed. 100% unit test pass.
</commit_message>
<xml_diff>
--- a/examples/searchcommands_app/Test-Performance.xlsx
+++ b/examples/searchcommands_app/Test-Performance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="5960" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SCPV1-1.3" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="25">
   <si>
     <t>Execution costs</t>
   </si>
@@ -108,10 +108,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;MB&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,29 +184,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -473,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView showRuler="0" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,14 +502,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -780,12 +792,12 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B23">
@@ -794,23 +806,23 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <f>35721690/(1024*1024)</f>
         <v>34.066858291625977</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="A26" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1093,12 +1105,12 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B48">
@@ -1106,19 +1118,334 @@
         <v>4.6319999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="3">
         <f>35721955/(1024*1024)</f>
         <v>34.067111015319824</v>
       </c>
     </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>0.05</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1">
+        <v>500001</v>
+      </c>
+      <c r="F55" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>5.27</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>0.08</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>0.08</v>
+      </c>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>5.5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>5.32</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>5.32</v>
+      </c>
+      <c r="C65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>0.08</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>0.01</v>
+      </c>
+      <c r="C67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D67">
+        <v>7</v>
+      </c>
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>0.02</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>0.04</v>
+      </c>
+      <c r="C69" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71">
+        <v>5.6849999999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <f>AVERAGE(B20,B45,B71)</f>
+        <v>5.5393333333333326</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A52:F52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1126,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,14 +1470,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1416,20 +1743,20 @@
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <f>33726832/(1024*1024)</f>
         <v>32.164413452148438</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="A24" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1671,7 +1998,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>0.02</v>
       </c>
       <c r="C40" t="s">
@@ -1713,32 +2040,971 @@
       <c r="A46" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="3">
         <f>33729512/(1024*1024)</f>
         <v>32.166969299316406</v>
       </c>
     </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>0.04</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>500001</v>
+      </c>
+      <c r="F52" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>7.03</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>0.09</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>0.09</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>7.24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>7.07</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>7.07</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>0.08</v>
+      </c>
+      <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>0.01</v>
+      </c>
+      <c r="C64" t="s">
+        <v>19</v>
+      </c>
+      <c r="D64">
+        <v>7</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>0.02</v>
+      </c>
+      <c r="C65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>0.04</v>
+      </c>
+      <c r="C66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68">
+        <v>7.43</v>
+      </c>
+      <c r="C68" s="6">
+        <f>B68 / 'SCPV1-1.3'!B45 - 1</f>
+        <v>0.36355294549458606</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71">
+        <f>6555/1000</f>
+        <v>6.5549999999999997</v>
+      </c>
+      <c r="C71" s="6">
+        <f>B71 / 'SCPV1-1.3'!B48 - 1</f>
+        <v>0.41515544041450791</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="3">
+        <f>33725994/(1024*1024)</f>
+        <v>32.163614273071289</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>0.05</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1">
+        <v>500001</v>
+      </c>
+      <c r="F78" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>5.61</v>
+      </c>
+      <c r="C79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>0.09</v>
+      </c>
+      <c r="C82" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>0.09</v>
+      </c>
+      <c r="C83" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>5.86</v>
+      </c>
+      <c r="C84" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>5.66</v>
+      </c>
+      <c r="C85" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>16</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>5.66</v>
+      </c>
+      <c r="C88" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>0.08</v>
+      </c>
+      <c r="C89" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+      <c r="E89" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>0.01</v>
+      </c>
+      <c r="C90" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90">
+        <v>7</v>
+      </c>
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>0.02</v>
+      </c>
+      <c r="C91" t="s">
+        <v>20</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>0.04</v>
+      </c>
+      <c r="C92" t="s">
+        <v>21</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>22</v>
+      </c>
+      <c r="B94">
+        <v>6.0460000000000003</v>
+      </c>
+      <c r="C94">
+        <f>B94-'SCPV1-1.3'!B71</f>
+        <v>0.36100000000000065</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C95" s="6">
+        <f>C94/'SCPV1-1.3'!B71</f>
+        <v>6.3500439753738022E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="9"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s">
+        <v>3</v>
+      </c>
+      <c r="E103" t="s">
+        <v>4</v>
+      </c>
+      <c r="F103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>0.05</v>
+      </c>
+      <c r="C104" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104" s="1">
+        <v>500001</v>
+      </c>
+      <c r="F104" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>5.03</v>
+      </c>
+      <c r="C105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>0.11</v>
+      </c>
+      <c r="C108" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>0.11</v>
+      </c>
+      <c r="C109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>5.28</v>
+      </c>
+      <c r="C110" t="s">
+        <v>13</v>
+      </c>
+      <c r="D110">
+        <v>2</v>
+      </c>
+      <c r="E110" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>5.08</v>
+      </c>
+      <c r="C111" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
+        <v>8</v>
+      </c>
+      <c r="F111" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>16</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>5.08</v>
+      </c>
+      <c r="C114" t="s">
+        <v>17</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114" t="s">
+        <v>8</v>
+      </c>
+      <c r="F114" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C115" t="s">
+        <v>18</v>
+      </c>
+      <c r="D115">
+        <v>2</v>
+      </c>
+      <c r="E115" t="s">
+        <v>8</v>
+      </c>
+      <c r="F115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>0.01</v>
+      </c>
+      <c r="C116" t="s">
+        <v>19</v>
+      </c>
+      <c r="D116">
+        <v>7</v>
+      </c>
+      <c r="E116" t="s">
+        <v>8</v>
+      </c>
+      <c r="F116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>0.02</v>
+      </c>
+      <c r="C117" t="s">
+        <v>20</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117" t="s">
+        <v>8</v>
+      </c>
+      <c r="F117" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>0.04</v>
+      </c>
+      <c r="C118" t="s">
+        <v>21</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118" t="s">
+        <v>8</v>
+      </c>
+      <c r="F118" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>22</v>
+      </c>
+      <c r="B120">
+        <v>5.4859999999999998</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A101:F101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView showRuler="0" topLeftCell="A88" zoomScale="81" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
@@ -1746,14 +3012,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1993,7 +3259,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>0.02</v>
       </c>
@@ -2010,7 +3276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -2027,100 +3293,123 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <f>1 - 6.88/AVERAGE(7.81,8.22)</f>
+        <v>0.14160948222083602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="8">
         <v>7.8140000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>1</v>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>0.02</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1">
+        <v>500001</v>
+      </c>
+      <c r="F29" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B30">
-        <v>0.02</v>
+        <v>7.84</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D30">
         <v>11</v>
       </c>
-      <c r="E30" s="1">
-        <v>500001</v>
+      <c r="E30" t="s">
+        <v>8</v>
       </c>
       <c r="F30" s="1">
         <v>500001</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B31">
-        <v>7.84</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D31">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="1">
-        <v>500001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2134,10 +3423,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2154,7 +3443,7 @@
         <v>0.17</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -2168,13 +3457,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B35">
-        <v>0.17</v>
+        <v>7.8</v>
       </c>
       <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35">
         <v>12</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -2185,13 +3474,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36">
-        <v>7.8</v>
+        <v>7.86</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D36">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -2202,13 +3491,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37">
-        <v>7.86</v>
+        <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
@@ -2222,10 +3511,10 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D38">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
@@ -2236,13 +3525,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39">
-        <v>0</v>
+        <v>7.85</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
@@ -2253,13 +3542,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40">
-        <v>7.85</v>
+        <v>0.1</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D40">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
@@ -2270,13 +3559,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D41">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -2290,10 +3579,10 @@
         <v>0.02</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D42">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
         <v>8</v>
@@ -2304,64 +3593,981 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B43">
+        <v>0.04</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="8">
+        <v>8.2219999999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54">
         <v>0.02</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>11</v>
+      </c>
+      <c r="E54" s="1">
+        <v>500001</v>
+      </c>
+      <c r="F54" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>6.25</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>0.08</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>0.08</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>6.15</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60">
+        <v>12</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>6.27</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>6.27</v>
+      </c>
+      <c r="C64" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>0.09</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65">
+        <v>12</v>
+      </c>
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>0.02</v>
+      </c>
+      <c r="C66" t="s">
+        <v>19</v>
+      </c>
+      <c r="D66">
+        <v>15</v>
+      </c>
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>0.02</v>
+      </c>
+      <c r="C67" t="s">
         <v>20</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>8</v>
-      </c>
-      <c r="F43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44">
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" s="8">
+        <v>6.4779999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B74" s="6">
+        <f>6.48/5.449 - 1</f>
+        <v>0.1892090291796662</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B75" s="6">
+        <f>6.25/'SCPV1-1.3'!B30 - 1</f>
+        <v>0.23031496062992129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>0.02</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81">
+        <v>11</v>
+      </c>
+      <c r="E81" s="1">
+        <v>500001</v>
+      </c>
+      <c r="F81" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82">
+        <v>11</v>
+      </c>
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>0.09</v>
+      </c>
+      <c r="C85" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>0.09</v>
+      </c>
+      <c r="C86" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>5.01</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87">
+        <v>12</v>
+      </c>
+      <c r="E87" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>5.13</v>
+      </c>
+      <c r="C88" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89">
+        <v>4</v>
+      </c>
+      <c r="E89" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>5.13</v>
+      </c>
+      <c r="C91" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91">
+        <v>11</v>
+      </c>
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>0.1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>18</v>
+      </c>
+      <c r="D92">
+        <v>12</v>
+      </c>
+      <c r="E92" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>0.01</v>
+      </c>
+      <c r="C93" t="s">
+        <v>19</v>
+      </c>
+      <c r="D93">
+        <v>13</v>
+      </c>
+      <c r="E93" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>0.02</v>
+      </c>
+      <c r="C94" t="s">
+        <v>20</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B95">
         <v>0.04</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C95" t="s">
         <v>21</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>8</v>
-      </c>
-      <c r="F44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>22</v>
       </c>
-      <c r="B46">
-        <v>8.2219999999999995</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="B97" s="8">
+        <v>5.3419999999999996</v>
+      </c>
+      <c r="C97" s="8">
+        <f>B97-'SCPV1-1.3'!B76</f>
+        <v>-0.19733333333333292</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C98" s="6">
+        <f>C97/'SCPV1-1.3'!B76</f>
+        <v>-3.5624022144662343E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="9"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s">
+        <v>3</v>
+      </c>
+      <c r="E106" t="s">
+        <v>4</v>
+      </c>
+      <c r="F106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>0.02</v>
+      </c>
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107">
+        <v>11</v>
+      </c>
+      <c r="E107" s="1">
+        <v>500001</v>
+      </c>
+      <c r="F107" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>4.34</v>
+      </c>
+      <c r="C108" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108">
+        <v>11</v>
+      </c>
+      <c r="E108" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" s="1">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110" t="s">
+        <v>10</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>0.08</v>
+      </c>
+      <c r="C111" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
+        <v>8</v>
+      </c>
+      <c r="F111" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>0.08</v>
+      </c>
+      <c r="C112" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="C113" t="s">
+        <v>13</v>
+      </c>
+      <c r="D113">
+        <v>12</v>
+      </c>
+      <c r="E113" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="C114" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114" t="s">
+        <v>8</v>
+      </c>
+      <c r="F114" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+      <c r="E115" t="s">
+        <v>8</v>
+      </c>
+      <c r="F115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116" t="s">
+        <v>16</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
+        <v>8</v>
+      </c>
+      <c r="F116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="C117" t="s">
+        <v>17</v>
+      </c>
+      <c r="D117">
+        <v>11</v>
+      </c>
+      <c r="E117" t="s">
+        <v>8</v>
+      </c>
+      <c r="F117" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>0.1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>18</v>
+      </c>
+      <c r="D118">
+        <v>12</v>
+      </c>
+      <c r="E118" t="s">
+        <v>8</v>
+      </c>
+      <c r="F118" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>0.02</v>
+      </c>
+      <c r="C119" t="s">
+        <v>19</v>
+      </c>
+      <c r="D119">
+        <v>11</v>
+      </c>
+      <c r="E119" t="s">
+        <v>8</v>
+      </c>
+      <c r="F119" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>0.02</v>
+      </c>
+      <c r="C120" t="s">
+        <v>20</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120" t="s">
+        <v>8</v>
+      </c>
+      <c r="F120" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>0.04</v>
+      </c>
+      <c r="C121" t="s">
+        <v>21</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121" t="s">
+        <v>8</v>
+      </c>
+      <c r="F121" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>22</v>
+      </c>
+      <c r="B123">
+        <v>4.5670000000000002</v>
+      </c>
+      <c r="C123" s="8">
+        <f>B123-'SCPV1-1.3'!B45</f>
+        <v>-0.88199999999999967</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C124" s="6">
+        <f>C123/'SCPV1-1.3'!B45</f>
+        <v>-0.16186456230501003</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A27:F27"/>
+  <mergeCells count="5">
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A104:F104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Removed some extraneous code and a TODO
</commit_message>
<xml_diff>
--- a/examples/searchcommands_app/Test-Performance.xlsx
+++ b/examples/searchcommands_app/Test-Performance.xlsx
@@ -490,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A30" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -3001,13 +3001,13 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A106" zoomScale="81" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="36.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
@@ -4860,8 +4860,8 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C150" s="6">
-        <f>C149/'SCPV1-1.3'!B71</f>
-        <v>-0.32700087950747586</v>
+        <f>1 - C149/'SCPV1-1.3'!B45</f>
+        <v>1.3411635162415121</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>